<commit_message>
27/6: Se realizan pruebas
</commit_message>
<xml_diff>
--- a/DescargaDocumentosOC/oc_pruebas.xlsx
+++ b/DescargaDocumentosOC/oc_pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldelgado\Desktop\0_proyectos\AYF\descargas_adj_oc\descargas_adj_oc\DescargaDocumentosOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6FA032-F82E-49DC-BC47-1513F1D32405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DDE2D9-9B28-49AB-A365-800293E7EB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,32 +370,207 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>4300012625</v>
+        <v>4300012630</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>4300012626</v>
+        <v>4300012631</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4300012627</v>
+        <v>4300012632</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4300012628</v>
+        <v>4300012633</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4300012629</v>
+        <v>4300012634</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4300012630</v>
+        <v>4300012635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4300012636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4300012637</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4300012638</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4300012639</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4300012640</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4300012641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4300012642</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>4300012643</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4300012644</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>4300012645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>4300012646</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>4300012647</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>4300012648</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>4300012649</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>4300012650</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>4300012651</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>4300012652</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>4300012653</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>4300012654</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>4300012655</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>4300012656</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>4300012657</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>4300012658</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>4300012659</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>4300012660</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4300012661</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>4300012662</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>4300012663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>4300012664</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>4300012665</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>4300012666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>4300012667</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>4300012668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>4300012669</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>4300012670</v>
       </c>
     </row>
   </sheetData>

</xml_diff>